<commit_message>
Prepare for a new PEST calibration of the upper part of the Long Tom basin. CW3M_UpperWRB.envx - Use Reporter.xml.  There isn't any Reporter_UpperWRB.xml. PEST_FRN7/flow2010.ic, HRU_PEST_FRN7.dbf, IDU_PEST_FRN7.dbf, Reach_PEST_FRN7.dbf - From a new spinup of FRN7.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BBEF60-1F44-4516-8694-82A4989416FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A1B130-E8E6-4131-B84B-A7E357FB0655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34065" yWindow="-6540" windowWidth="20175" windowHeight="10770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All WRB gages" sheetId="2" r:id="rId1"/>
     <sheet name="South Santiam" sheetId="4" r:id="rId2"/>
     <sheet name="Coast Fork" sheetId="5" r:id="rId3"/>
+    <sheet name="Long Tom" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="blanks" localSheetId="0">'All WRB gages'!$A$1:$J$78</definedName>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
   <si>
     <t>blanks</t>
   </si>
@@ -616,6 +617,66 @@
   </si>
   <si>
     <t>gage area / comid area</t>
+  </si>
+  <si>
+    <t>FRN7 pour point</t>
+  </si>
+  <si>
+    <t>Long Tom River near Alvadore below FRN</t>
+  </si>
+  <si>
+    <t>Long Tom at Monroe</t>
+  </si>
+  <si>
+    <t>Long Tom outlet into the Willamette</t>
+  </si>
+  <si>
+    <r>
+      <t>44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 07'25"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>123°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 17'55"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> LONG TOM RIVER NEAR NOTI 23763161</t>
   </si>
 </sst>
 </file>
@@ -748,11 +809,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="blanks" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="blanks_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="blanks_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="blanks" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1079,8 +1140,8 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69:J69"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3734,8 +3795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3094A183-0AC5-4077-AB1E-2FD8B3D14819}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3931,4 +3992,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639DAE21-C1F0-4C54-8DDD-2086C4EA615A}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="11" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="10" style="11" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="12" max="14" width="8.44140625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="37.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="25" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>14166500</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="11">
+        <v>23763161</v>
+      </c>
+      <c r="E2" s="11">
+        <v>23514.608</v>
+      </c>
+      <c r="L2" s="9">
+        <v>89.3</v>
+      </c>
+      <c r="M2" s="11">
+        <f>E2/258.9988</f>
+        <v>90.790412928554105</v>
+      </c>
+      <c r="N2" s="10">
+        <f t="shared" ref="N2" si="0">L2/M2</f>
+        <v>0.98358402742669582</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="11">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11">
+        <v>23763141</v>
+      </c>
+      <c r="E3" s="11">
+        <v>64568.691200000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>14169000</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="11">
+        <v>23763139</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="L4" s="11">
+        <v>252</v>
+      </c>
+      <c r="M4" s="11">
+        <f>E3/258.9988</f>
+        <v>249.30112108627529</v>
+      </c>
+      <c r="N4" s="10">
+        <f t="shared" ref="N4" si="1">L4/M4</f>
+        <v>1.0108257792903816</v>
+      </c>
+      <c r="O4" s="9">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>14170000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="11">
+        <v>35</v>
+      </c>
+      <c r="D5" s="11">
+        <v>23763077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="11">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11">
+        <v>23763069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prepare for a new PEST calibration of the Marys basin.  Consolidate the skill spreadsheets. CW3M_Marys.envx, CW3M_PEST_Marys23.envx - Update to current conventions. Marys/flow2010.ic, HRU_Marys.dbf, IDU_Marys.dbf, Reach_Marys.dbf - From a new spinup. Add FLOWreports_Marys.xml. Combine the skill spreadsheets for the various basins into a new Skill.xlsx spreadsheet.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A1B130-E8E6-4131-B84B-A7E357FB0655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E045E9-0FCB-4D51-8263-427968AFB61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34065" yWindow="-6540" windowWidth="20175" windowHeight="10770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34065" yWindow="-6540" windowWidth="20175" windowHeight="10770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All WRB gages" sheetId="2" r:id="rId1"/>
     <sheet name="South Santiam" sheetId="4" r:id="rId2"/>
     <sheet name="Coast Fork" sheetId="5" r:id="rId3"/>
     <sheet name="Long Tom" sheetId="6" r:id="rId4"/>
+    <sheet name="McKenzie" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="blanks" localSheetId="0">'All WRB gages'!$A$1:$J$78</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="216">
   <si>
     <t>blanks</t>
   </si>
@@ -678,15 +679,151 @@
   <si>
     <t xml:space="preserve"> LONG TOM RIVER NEAR NOTI 23763161</t>
   </si>
+  <si>
+    <t>gage number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reach </t>
+  </si>
+  <si>
+    <t>IDU_ID</t>
+  </si>
+  <si>
+    <t>HRU_ID</t>
+  </si>
+  <si>
+    <t># of IDUs</t>
+  </si>
+  <si>
+    <t>HBVCALIB area, m2</t>
+  </si>
+  <si>
+    <t>HBVCALIB area, sq. mi.</t>
+  </si>
+  <si>
+    <t>NAD27 lat</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>UTM zone 10T easting</t>
+  </si>
+  <si>
+    <t>northing</t>
+  </si>
+  <si>
+    <t>elev</t>
+  </si>
+  <si>
+    <t>gage drainage area, sq. mi.</t>
+  </si>
+  <si>
+    <t>gage area: HBVCALIB area</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ngs.noaa.gov/NCAT</t>
+  </si>
+  <si>
+    <t>ClearLake46</t>
+  </si>
+  <si>
+    <t>44deg 21' 40"</t>
+  </si>
+  <si>
+    <t>121deg 59' 40"</t>
+  </si>
+  <si>
+    <t>3015.32 ft</t>
+  </si>
+  <si>
+    <t>MCKENZIE RIVER AT OUTLET OF CLEAR LAKE, OR</t>
+  </si>
+  <si>
+    <t>Smith47</t>
+  </si>
+  <si>
+    <t>44deg 20' 05"</t>
+  </si>
+  <si>
+    <t>122 deg 02' 45"</t>
+  </si>
+  <si>
+    <t>2610 ft</t>
+  </si>
+  <si>
+    <t>SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRNGS</t>
+  </si>
+  <si>
+    <t>SFork48</t>
+  </si>
+  <si>
+    <t>44deg 02' 50"</t>
+  </si>
+  <si>
+    <t>122deg 13' 00"</t>
+  </si>
+  <si>
+    <t>1709.51 ft</t>
+  </si>
+  <si>
+    <t>SO FK MCKENZIE RIVER ABV COUGAR LAKE NR RAINBOW</t>
+  </si>
+  <si>
+    <t>above Penny Cr 23774625, below French Pete Cr 23773153</t>
+  </si>
+  <si>
+    <t>Lookout49</t>
+  </si>
+  <si>
+    <t>44deg 12' 35"</t>
+  </si>
+  <si>
+    <t>122deg 15' 20"</t>
+  </si>
+  <si>
+    <t>1377.76 ft</t>
+  </si>
+  <si>
+    <t>LOOKOUT CREEK NEAR BLUE RIVER</t>
+  </si>
+  <si>
+    <t>BLU9 (+Lookout49)</t>
+  </si>
+  <si>
+    <t>1056.53 ft</t>
+  </si>
+  <si>
+    <t>BLUE RIVER AT BLUE RIVER</t>
+  </si>
+  <si>
+    <t>below Quartz Cr, above Simmons Cr</t>
+  </si>
+  <si>
+    <t>Mohawk25</t>
+  </si>
+  <si>
+    <t>44deg 05' 35"</t>
+  </si>
+  <si>
+    <t>122deg 57' 22"</t>
+  </si>
+  <si>
+    <t>MOHAWK RIVER NEAR SPRINGFIELD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -716,7 +853,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +872,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -748,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -791,6 +934,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3998,7 +4155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639DAE21-C1F0-4C54-8DDD-2086C4EA615A}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -4168,4 +4325,384 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65080B93-6114-467E-93BC-27671F963286}">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28">
+        <v>14158500</v>
+      </c>
+      <c r="B2" s="28">
+        <v>23773373</v>
+      </c>
+      <c r="D2" s="28">
+        <v>3069</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="28">
+        <v>508</v>
+      </c>
+      <c r="G2" s="29">
+        <v>88119000</v>
+      </c>
+      <c r="H2" s="30">
+        <f>G2/2589988</f>
+        <v>34.022937558011854</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="28">
+        <v>580131</v>
+      </c>
+      <c r="L2" s="28">
+        <v>4912257</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" s="28">
+        <v>92.4</v>
+      </c>
+      <c r="O2" s="31">
+        <f>(N2*2589988)/G2</f>
+        <v>2.7158148776086883</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28">
+        <v>14158790</v>
+      </c>
+      <c r="B3" s="28">
+        <v>23773393</v>
+      </c>
+      <c r="C3" s="28">
+        <v>52940</v>
+      </c>
+      <c r="D3" s="28">
+        <v>3036</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="28">
+        <v>229</v>
+      </c>
+      <c r="G3" s="29">
+        <v>42488300</v>
+      </c>
+      <c r="H3" s="30">
+        <f t="shared" ref="H3:H7" si="0">G3/2589988</f>
+        <v>16.404825041660423</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" s="28">
+        <v>576070</v>
+      </c>
+      <c r="L3" s="28">
+        <v>4909277</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="N3" s="28">
+        <v>15.6</v>
+      </c>
+      <c r="O3" s="31">
+        <f t="shared" ref="O3:O7" si="1">(N3*2589988)/G3</f>
+        <v>0.95093973635094831</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28">
+        <v>14159200</v>
+      </c>
+      <c r="B4" s="28">
+        <v>23773037</v>
+      </c>
+      <c r="C4" s="28">
+        <v>30677</v>
+      </c>
+      <c r="D4" s="28">
+        <v>1785</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="28">
+        <v>2229</v>
+      </c>
+      <c r="G4" s="29">
+        <v>404283000</v>
+      </c>
+      <c r="H4" s="30">
+        <f t="shared" si="0"/>
+        <v>156.09454561179433</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="K4" s="28">
+        <v>562755</v>
+      </c>
+      <c r="L4" s="28">
+        <v>4877200</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="N4" s="28">
+        <v>160</v>
+      </c>
+      <c r="O4" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0250198004862929</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
+        <v>14161500</v>
+      </c>
+      <c r="B5" s="28">
+        <v>23773411</v>
+      </c>
+      <c r="C5" s="28">
+        <v>45726</v>
+      </c>
+      <c r="D5" s="28">
+        <v>2564</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="28">
+        <v>236</v>
+      </c>
+      <c r="G5" s="29">
+        <v>63516000</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" si="0"/>
+        <v>24.523665746713885</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="K5" s="28">
+        <v>559476</v>
+      </c>
+      <c r="L5" s="28">
+        <v>4895217</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="N5" s="28">
+        <v>24.1</v>
+      </c>
+      <c r="O5" s="31">
+        <f t="shared" si="1"/>
+        <v>0.98272420807355632</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
+        <v>14162200</v>
+      </c>
+      <c r="B6" s="28">
+        <v>23773405</v>
+      </c>
+      <c r="D6" s="28">
+        <v>2400</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="28">
+        <v>763</v>
+      </c>
+      <c r="G6" s="29">
+        <v>164367000</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="0"/>
+        <v>63.462456196708246</v>
+      </c>
+      <c r="I6" s="28">
+        <v>44.162348190000003</v>
+      </c>
+      <c r="J6" s="28">
+        <v>-122.3331192</v>
+      </c>
+      <c r="K6" s="28">
+        <v>553322</v>
+      </c>
+      <c r="L6" s="28">
+        <v>4889905</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="28">
+        <v>87.7</v>
+      </c>
+      <c r="O6" s="31">
+        <f>N6/(H5+H6)</f>
+        <v>0.99674810143801862</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="33">
+        <v>14165000</v>
+      </c>
+      <c r="B7" s="28">
+        <v>23773513</v>
+      </c>
+      <c r="C7" s="28">
+        <v>34180</v>
+      </c>
+      <c r="D7" s="28">
+        <v>2021</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="28">
+        <v>2088</v>
+      </c>
+      <c r="G7" s="29">
+        <v>463631000</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" si="0"/>
+        <v>179.00893749314668</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="K7" s="28">
+        <v>503513</v>
+      </c>
+      <c r="L7" s="28">
+        <v>4881993</v>
+      </c>
+      <c r="M7" s="28">
+        <v>442.47</v>
+      </c>
+      <c r="N7" s="28">
+        <v>177</v>
+      </c>
+      <c r="O7" s="31">
+        <f t="shared" si="1"/>
+        <v>0.98877744585672656</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust Q_DISCHARG at the Marys R gage in Philomath to account for the difference between the gage drainage area and the CW3M cumulative area for that reach. I don't know why the USGS gage drainage area is larger than the CW3M cumulative area. FLOWreports_Marys.xml - Adjust Q_DISCHARG up by 5% to compare with gage data.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E045E9-0FCB-4D51-8263-427968AFB61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066A368B-2A53-452B-A144-69288AB75F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34065" yWindow="-6540" windowWidth="20175" windowHeight="10770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1452" yWindow="948" windowWidth="20172" windowHeight="10776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All WRB gages" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Coast Fork" sheetId="5" r:id="rId3"/>
     <sheet name="Long Tom" sheetId="6" r:id="rId4"/>
     <sheet name="McKenzie" sheetId="7" r:id="rId5"/>
+    <sheet name="Marys" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="blanks" localSheetId="0">'All WRB gages'!$A$1:$J$78</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="220">
   <si>
     <t>blanks</t>
   </si>
@@ -814,6 +815,18 @@
   <si>
     <t>MOHAWK RIVER NEAR SPRINGFIELD</t>
   </si>
+  <si>
+    <t>44°31'30.00"</t>
+  </si>
+  <si>
+    <t>123°20'02.40</t>
+  </si>
+  <si>
+    <t>44.5250</t>
+  </si>
+  <si>
+    <t>Marys River outlet into the Willamette</t>
+  </si>
 </sst>
 </file>
 
@@ -825,7 +838,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -851,6 +864,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -891,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -948,6 +968,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,9 +1320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4156,7 +4180,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4331,7 +4355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65080B93-6114-467E-93BC-27671F963286}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -4705,4 +4729,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145E1DF5-DEC5-41B1-B4B4-7F575AEAE5B0}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>14171000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>23762895</v>
+      </c>
+      <c r="E2" s="11">
+        <v>39212.8416</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="I2">
+        <v>123.334</v>
+      </c>
+      <c r="J2">
+        <v>473459</v>
+      </c>
+      <c r="K2">
+        <v>4930240</v>
+      </c>
+      <c r="L2">
+        <v>159</v>
+      </c>
+      <c r="M2" s="11">
+        <f>E2/258.9988</f>
+        <v>151.40163429328629</v>
+      </c>
+      <c r="N2" s="10">
+        <f t="shared" ref="N2" si="0">L2/M2</f>
+        <v>1.0501868143113609</v>
+      </c>
+      <c r="O2">
+        <v>224.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="21">
+        <v>23</v>
+      </c>
+      <c r="D3" s="21">
+        <v>23762881</v>
+      </c>
+      <c r="E3" s="21">
+        <v>77883.1872</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>14166500</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11">
+        <v>23763161</v>
+      </c>
+      <c r="E5" s="11">
+        <v>23514.608</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="L5" s="9">
+        <v>89.3</v>
+      </c>
+      <c r="M5" s="11">
+        <f>E5/258.9988</f>
+        <v>90.790412928554105</v>
+      </c>
+      <c r="N5" s="10">
+        <f t="shared" ref="N5" si="1">L5/M5</f>
+        <v>0.98358402742669582</v>
+      </c>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="11">
+        <v>7</v>
+      </c>
+      <c r="D6" s="11">
+        <v>23763141</v>
+      </c>
+      <c r="E6" s="11">
+        <v>64568.691200000001</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>14169000</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11">
+        <v>23763139</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="L7" s="11">
+        <v>252</v>
+      </c>
+      <c r="M7" s="11">
+        <f>E6/258.9988</f>
+        <v>249.30112108627529</v>
+      </c>
+      <c r="N7" s="10">
+        <f t="shared" ref="N7" si="2">L7/M7</f>
+        <v>1.0108257792903816</v>
+      </c>
+      <c r="O7" s="9">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>14170000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="11">
+        <v>35</v>
+      </c>
+      <c r="D8" s="11">
+        <v>23763077</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="11">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11">
+        <v>23763069</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add logic to support the use of basin-specific water rights data. Flow.xml - Add alternate_pod_table and alternate_pou_table fields to the WaterRights block. WaterRights.cpp, .h - Allow for {studyAreaName} in the input strings for pod_table and pou_table. Implement the alternate_pod_table and alternate_pou_fields. Add members m_altPodTablePath and m_altPouTablePath to class AltWaterMaster. STMengine.cpp - Correct a comment.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Gages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066A368B-2A53-452B-A144-69288AB75F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F6921D-F0B5-468B-8A5A-9D9A4B4F7847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="948" windowWidth="20172" windowHeight="10776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All WRB gages" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="221">
   <si>
     <t>blanks</t>
   </si>
@@ -827,6 +827,9 @@
   <si>
     <t>Marys River outlet into the Willamette</t>
   </si>
+  <si>
+    <t>Outlet of Muddy Creek into the Marys</t>
+  </si>
 </sst>
 </file>
 
@@ -836,7 +839,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -954,14 +957,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4733,10 +4736,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145E1DF5-DEC5-41B1-B4B4-7F575AEAE5B0}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4831,7 +4834,7 @@
       <c r="L2">
         <v>159</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="9">
         <f>E2/258.9988</f>
         <v>151.40163429328629</v>
       </c>
@@ -4843,37 +4846,36 @@
         <v>224.01</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="21">
-        <v>23</v>
-      </c>
-      <c r="D3" s="21">
-        <v>23762881</v>
-      </c>
-      <c r="E3" s="21">
-        <v>77883.1872</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3">
+        <v>23762959</v>
+      </c>
+      <c r="E3" s="11">
+        <v>31856.486400000002</v>
+      </c>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="6"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="B4" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="21">
+        <v>23</v>
+      </c>
+      <c r="D4" s="21">
+        <v>23762881</v>
+      </c>
+      <c r="E4" s="21">
+        <v>77883.1872</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="23"/>
@@ -4885,126 +4887,123 @@
       <c r="N4" s="24"/>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>14166500</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11">
         <v>23763161</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E6" s="11">
         <v>23514.608</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="L5" s="9">
-        <v>89.3</v>
-      </c>
-      <c r="M5" s="11">
-        <f>E5/258.9988</f>
-        <v>90.790412928554105</v>
-      </c>
-      <c r="N5" s="10">
-        <f t="shared" ref="N5" si="1">L5/M5</f>
-        <v>0.98358402742669582</v>
-      </c>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="11">
-        <v>7</v>
-      </c>
-      <c r="D6" s="11">
-        <v>23763141</v>
-      </c>
-      <c r="E6" s="11">
-        <v>64568.691200000001</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+      <c r="L6" s="9">
+        <v>89.3</v>
+      </c>
+      <c r="M6" s="11">
+        <f>E6/258.9988</f>
+        <v>90.790412928554105</v>
+      </c>
+      <c r="N6" s="10">
+        <f t="shared" ref="N6" si="1">L6/M6</f>
+        <v>0.98358402742669582</v>
+      </c>
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14169000</v>
-      </c>
       <c r="B7" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="11"/>
+        <v>164</v>
+      </c>
+      <c r="C7" s="11">
+        <v>7</v>
+      </c>
       <c r="D7" s="11">
-        <v>23763139</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>169</v>
-      </c>
+        <v>23763141</v>
+      </c>
+      <c r="E7" s="11">
+        <v>64568.691200000001</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-      <c r="L7" s="11">
-        <v>252</v>
-      </c>
-      <c r="M7" s="11">
-        <f>E6/258.9988</f>
-        <v>249.30112108627529</v>
-      </c>
-      <c r="N7" s="10">
-        <f t="shared" ref="N7" si="2">L7/M7</f>
-        <v>1.0108257792903816</v>
-      </c>
-      <c r="O7" s="9">
-        <v>332</v>
-      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>14170000</v>
-      </c>
-      <c r="B8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="11">
-        <v>35</v>
-      </c>
+        <v>14169000</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11">
-        <v>23763077</v>
+        <v>23763139</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>169</v>
+      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="L8" s="11">
+        <v>252</v>
+      </c>
+      <c r="M8" s="11">
+        <f>E7/258.9988</f>
+        <v>249.30112108627529</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" ref="N8" si="2">L8/M8</f>
+        <v>1.0108257792903816</v>
+      </c>
+      <c r="O8" s="9">
+        <v>332</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>14170000</v>
+      </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="11">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D9" s="11">
-        <v>23763069</v>
+        <v>23763077</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -5016,6 +5015,26 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="11">
+        <v>24</v>
+      </c>
+      <c r="D10" s="11">
+        <v>23763069</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>